<commit_message>
Done 1 - 2 - 3
</commit_message>
<xml_diff>
--- a/ListHandOver/Training_User.xlsx
+++ b/ListHandOver/Training_User.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SiVi CODE\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ThuyHV\Study\Node-JS\ListHandOver\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="ListHandOver" sheetId="1" r:id="rId1"/>
     <sheet name="Lập trình javascript căn bản" sheetId="4" r:id="rId2"/>
     <sheet name="Cấu trúc lập trình" sheetId="5" r:id="rId3"/>
     <sheet name="Function, Expression, methods" sheetId="6" r:id="rId4"/>
+    <sheet name=" Lập trình theo chuẩn ES5" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="216">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -1237,6 +1238,236 @@
   </si>
   <si>
     <t>Lặp FUNCTION</t>
+  </si>
+  <si>
+    <t>Function expressions</t>
+  </si>
+  <si>
+    <t>Có thể khai báo hàm như một biểu thức, tương tự khai báo một biến.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Có thể khai báo một biểu thức hàm mà không cần đặt tên cho hàm.</t>
+  </si>
+  <si>
+    <t>Anonymous functions</t>
+  </si>
+  <si>
+    <t>Khai báo hàm mà không cần tên hàm vi diệu sương sương thôi. Anonymous functions có thể khai báo hàm mà không cần từ khóa là FUNCTION.</t>
+  </si>
+  <si>
+    <t>Lambda functions</t>
+  </si>
+  <si>
+    <t>Lưu ý: Dùng Anonymous functions:</t>
+  </si>
+  <si>
+    <t>phải định nghĩa function trước rồi mới dùng. Không thể gọi thực thi trước rồi mới định nghĩa Function.</t>
+  </si>
+  <si>
+    <t>Có thể thêm tên cho function nhưng không thể gọi thực thi bằng tên function.</t>
+  </si>
+  <si>
+    <t>Viết Anonymous functions bằng cách ngắn gọn hơn</t>
+  </si>
+  <si>
+    <t>Như ví dụ thì dog1 được viết lại từ dog.</t>
+  </si>
+  <si>
+    <t>Generator functions</t>
+  </si>
+  <si>
+    <t>Là một Function được thực thi nhiều lần mà: số lượng biến, giá trị biến, trạng thái các thành phần của hàm..v..v đều được lưu lại sau mỗi phiên sử dụng. Và có thể dùng tiếp tại 1 phiên gọi tiếp theo.</t>
+  </si>
+  <si>
+    <t>Lấy 1 ví dụ như sau:</t>
+  </si>
+  <si>
+    <r>
+      <t>Tại đây có dùng</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> console.log(i) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nên có log ra cho mình xem giá trị tăng của i</t>
+    </r>
+  </si>
+  <si>
+    <t>Nếu chỉ muốn coi thằng i tăng tới 2 thì có thể if ở đây</t>
+  </si>
+  <si>
+    <t>Giờ không dùng if trong vòng lặp mà muốn dừng lại coi thì thử dùng Generator functions, từ cái hàm ở trên sửa lại như bên dưới</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ở đây phải đặt thêm 1 cái biến </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>generator</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> để kêu cái hàm ra</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>generator.next();</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Được gọi nó chạy tới hàm loopByN thực thi đến khi gặp yield thì dừng lại rồi giá trị i lúc đầu 0 i++ lên = 1 nhớ ở đó</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>generator.next();</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> được gọi lần 2 sau cái chổ "xử lý gì đó khác" dù gọi lại là nó chạy vô hàm loopByN theo suy nghỉ thông thường thì chạy lại từ đầu cái vòng lặp nhưng KHÔNG</t>
+    </r>
+  </si>
+  <si>
+    <t>Khi nảy nhớ là 1 thì giờ i là 1 chớ không phải 0 đâu nhé.</t>
+  </si>
+  <si>
+    <t>Cứ thế cứ gọi next là nó lại bay vô hàm rồi gặp yield là nó lại tạm dừng. Có thể dùng return để kết thúc hàm.</t>
+  </si>
+  <si>
+    <t>Một số function có sẵn trong Javascript</t>
+  </si>
+  <si>
+    <t>Với số</t>
+  </si>
+  <si>
+    <t>toFixed() hoặc toFixed(n) : Làm tròn tới n chữ số thập phân, không có n thì bỏ phần làm tròn</t>
+  </si>
+  <si>
+    <t>abs(num) : Trả về trị tuyệt đối của num</t>
+  </si>
+  <si>
+    <t>Với chữ</t>
+  </si>
+  <si>
+    <t>toLowerCase( ) : Trả về chuỗi ký tự thường</t>
+  </si>
+  <si>
+    <t>toUpperCase() : Trả về chuỗi ký tự in hoa</t>
+  </si>
+  <si>
+    <t>length : trả về độ dài của chuỗi</t>
+  </si>
+  <si>
+    <t>ĐÂY LÀ 1 TRONG SỐ RẤT ÍT HÀM CÓ SẴN  TRONG JAVASCRIPT CÒN RẤT NHIỀU HÀM CÓ SẴN KHÁC NỮA NHÉ!!!</t>
+  </si>
+  <si>
+    <t>Regular expression trong JavaScript</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biểu thức chính quy (regular expressions ) là các mẫu dùng để tìm kiếm các bộ kí tự được kết hợp với nhau trong các chuỗi kí tự. </t>
+  </si>
+  <si>
+    <t>Có thể dùng để validate form trước khi submit một bộ giá trị nào đó chẳng hạn như mail, số điện thoại, password v…v</t>
+  </si>
+  <si>
+    <t>Như ví dụ dưới đây tạo 1 biểu thức đơn giản để nhận lại 1 mảng giá trị số không liên tiếp của chuỗi.</t>
+  </si>
+  <si>
+    <t>Những quy tắc dùng trong Regular Expression (Regex)</t>
+  </si>
+  <si>
+    <t>Ký tự thường</t>
+  </si>
+  <si>
+    <t>Ký tự đặc biệt</t>
+  </si>
+  <si>
+    <t>Lặp</t>
+  </si>
+  <si>
+    <t>Khớp nhóm</t>
+  </si>
+  <si>
+    <t>Các phương pháp tạo Object</t>
+  </si>
+  <si>
+    <t>Sử dụng literal notation</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Object literal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> là kiểu cú pháp tạo object sử dụng cặp dấu ngoặc {} và bên trong đó là danh sách các property (thuộc tính) của object.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1246,7 +1477,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1327,6 +1558,30 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1452,7 +1707,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1505,6 +1760,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2344,6 +2603,771 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>419754</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>152634</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="4686954" cy="1676634"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>562479</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133448</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2857500"/>
+          <a:ext cx="3610479" cy="704948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219616</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>181240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4381500"/>
+          <a:ext cx="3877216" cy="1895740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>87183</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85987</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6972300"/>
+          <a:ext cx="10450383" cy="1876687"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>277625</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>19186</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9334500"/>
+          <a:ext cx="10031225" cy="971686"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>534155</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>181218</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="11201400"/>
+          <a:ext cx="5410955" cy="1743318"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>57924</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>85923</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="14097000"/>
+          <a:ext cx="5544324" cy="1419423"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>124863</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>9816</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="16211550"/>
+          <a:ext cx="7440063" cy="2086266"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>257977</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>123922</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="19431000"/>
+          <a:ext cx="5744377" cy="695422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>277029</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>57216</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="20535900"/>
+          <a:ext cx="5763429" cy="476316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>229398</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>38158</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="21526500"/>
+          <a:ext cx="5715798" cy="419158"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238924</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>104843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="22288500"/>
+          <a:ext cx="5725324" cy="485843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>219871</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>181041</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="23136225"/>
+          <a:ext cx="5706271" cy="476316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>363022</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>104913</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="25784175"/>
+          <a:ext cx="7678222" cy="990738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>10462</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>95763</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="27660600"/>
+          <a:ext cx="6716062" cy="3677163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581957</xdr:colOff>
+      <xdr:row>185</xdr:row>
+      <xdr:rowOff>181472</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="31861125"/>
+          <a:ext cx="6677957" cy="3562847"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>486694</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>114741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="35433000"/>
+          <a:ext cx="6582694" cy="3162741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>205</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>524799</xdr:colOff>
+      <xdr:row>221</xdr:row>
+      <xdr:rowOff>19474</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="39462075"/>
+          <a:ext cx="6620799" cy="3038899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>562904</xdr:colOff>
+      <xdr:row>242</xdr:row>
+      <xdr:rowOff>57610</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="42862500"/>
+          <a:ext cx="6658904" cy="3296110"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>245</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>534325</xdr:colOff>
+      <xdr:row>260</xdr:row>
+      <xdr:rowOff>143294</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="46672500"/>
+          <a:ext cx="6630325" cy="3000794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2610,10 +3634,10 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2626,41 +3650,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="26" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="26"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
@@ -4061,8 +5085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4405,8 +5429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K92" sqref="K92"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4526,14 +5550,283 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N244"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="J24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="B48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="B58" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B70" s="20"/>
+      <c r="C70" s="20"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="B73" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="K76" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="K77" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="84" spans="2:14">
+      <c r="B84" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="87" spans="2:14">
+      <c r="N87" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="88" spans="2:14">
+      <c r="N88" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="2:14">
+      <c r="N89" s="21" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="90" spans="2:14">
+      <c r="N90" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="91" spans="2:14">
+      <c r="N91" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B99" s="20"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="20"/>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="B101" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="B107" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="B113" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="B117" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="B121" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="23"/>
+      <c r="B128" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B130" s="20"/>
+      <c r="C130" s="20"/>
+      <c r="D130" s="20"/>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4">
+      <c r="A144" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="205" spans="2:2">
+      <c r="B205" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2">
+      <c r="B224" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="244" spans="2:2">
+      <c r="B244" t="s">
+        <v>212</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="20" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="B3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DONE 6 Làm việc với scope của variables
</commit_message>
<xml_diff>
--- a/ListHandOver/Training_User.xlsx
+++ b/ListHandOver/Training_User.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="ListHandOver" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Function, Expression, methods" sheetId="6" r:id="rId4"/>
     <sheet name=" Lập trình theo chuẩn ES5" sheetId="7" r:id="rId5"/>
     <sheet name="Kiến thức với mảng" sheetId="8" r:id="rId6"/>
+    <sheet name="Scope của variables" sheetId="9" r:id="rId7"/>
+    <sheet name="Làm việc với con trỏ this" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="311">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -1753,6 +1755,401 @@
       </rPr>
       <t>p Array: Array.prototype.slice(), Array.from()…</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Viết một hàm filterRange trả về mảng đã loại bỏ tất cả các giá trị ngoại trừ những giá trị nằm giữa giá trị from và to.</t>
+    </r>
+  </si>
+  <si>
+    <t>Xử lý dãy số</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Cho mảng số nguyên dương tăng (chưa được sắp xếp) khuyết 1 phần tử, tìm phần tử bị thiếu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Cho mảng số nguyên tính tổng các số nguyên là số chẳn.</t>
+    </r>
+  </si>
+  <si>
+    <t>Mảng đối tượng</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Cho mảng đối tượng học sinh lấy ra danh sách tên học sinh có tuổi lớn hơn k.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Cho mảng đối tượng nhân viên tính lương trung bình của cả công ty.</t>
+    </r>
+  </si>
+  <si>
+    <t>Tìm kiếm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Tìm kiếm toàn bộ mã thuộc phòng ban là giám đốc GD.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Tìm kiếm toàn bộ số nguyên tố trong mảng số nguyên.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Tìm kiếm toàn bộ nhân viên có lương từ 10 triệu trở lên.</t>
+    </r>
+  </si>
+  <si>
+    <t>Sắp xếp</t>
+  </si>
+  <si>
+    <t>Đệ quy</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Sắp xếp dãy số nguyên tăng</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Sắp xếp dãy số nguyên giảm</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Sắp xếp danh sách nhân viên theo thứ tự tăng về tuổi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Xây dựng chức năng đếm ngược chúc mừng năm mới.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bài 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Tìm số fibonacci thứ N.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cách sử dụng lớp Array: Array.prototype.slice(), Array.from()…</t>
+  </si>
+  <si>
+    <t>Array.prototype.slice()</t>
+  </si>
+  <si>
+    <t>Dùng để lấy số lượng phần tử của mảng từ vị trí start đến end (Tuy nhiên sẽ không lấy giá trị ở vị trí end)</t>
+  </si>
+  <si>
+    <t>Array.from()</t>
+  </si>
+  <si>
+    <t>Có thể tạo mảng từ một dữ liệu khác</t>
+  </si>
+  <si>
+    <t>Array.includes()</t>
+  </si>
+  <si>
+    <t>Kiểm tra sự tồn tại của item nằm trong mảng</t>
+  </si>
+  <si>
+    <t>Array.some()</t>
+  </si>
+  <si>
+    <t>Kiểm tra array có bất kỳ phần tử nào thỏa mãn 1 điều kiện nào đó</t>
+  </si>
+  <si>
+    <t>Array.every()</t>
+  </si>
+  <si>
+    <t>Kiểm tra toàn bộ phần tử array có thỏa mãn 1 điều kiện nào đó</t>
+  </si>
+  <si>
+    <t>Global scope</t>
+  </si>
+  <si>
+    <t>Các biến khai báo ngoài Function, biến đó được dùng chung cho các Function, có thể thay đổi giá trị của biến trong các Function.</t>
+  </si>
+  <si>
+    <t>Scope giới hạn của các biến khai báo với let, const</t>
+  </si>
+  <si>
+    <t>Ở global scope từ khóa var tạo ra thuộc tính mới cho global object (this), còn let thì không.</t>
+  </si>
+  <si>
+    <t>Các biến được khai báo var là function scope, nếu biến được khai báo trong một block scope thì biến đó cũng có thể truy cập được  bên ngoài.</t>
+  </si>
+  <si>
+    <t>Các biến được khai báo let là block cope, nếu biến được khai báo trong một block scope thì biến đó không thể truy cập được  bên ngoài.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Const tương tự let nhưng không được phép thay đổi giá trị </t>
+  </si>
+  <si>
+    <t>Scope của variables trong functions</t>
+  </si>
+  <si>
+    <t>Các biến khai báo var, let, const bên trong function scope thì không thể truy cập được bên ngoài function</t>
+  </si>
+  <si>
+    <t>Scope của variables trong block code</t>
+  </si>
+  <si>
+    <t>Đối với var sẽ chỉ giới hạn ở trong function scope nên nếu dùng var khai báo trong một block scope thì có thể truy cập bên ngoài được.</t>
+  </si>
+  <si>
+    <t>Tuy nhiên sử dụng let và const thì chỉ có thể truy cập được ở mức block scope.</t>
+  </si>
+  <si>
+    <t>Scope của variables trong Closure functions</t>
+  </si>
+  <si>
+    <t>Biến số nằm trong hàm có thể truy cập được từ một hàm nằm bên trong hàm đó</t>
+  </si>
+  <si>
+    <t>Tìm hiểu các cách binding(liên kết) giữa "this" với methods như: Implicit binding, Explicit binding, "new" binding, Lexical binding, default/window binding</t>
+  </si>
+  <si>
+    <t>Implicit binding</t>
   </si>
 </sst>
 </file>
@@ -2061,6 +2458,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2069,10 +2470,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4626,6 +5023,961 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>67705</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>47951</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="22098000"/>
+          <a:ext cx="7382905" cy="2333951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>115252</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>114662</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="25146000"/>
+          <a:ext cx="6820852" cy="2591162"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>96199</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>152767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28384500"/>
+          <a:ext cx="6801799" cy="2629267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>544277</xdr:colOff>
+      <xdr:row>183</xdr:row>
+      <xdr:rowOff>86136</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="32004000"/>
+          <a:ext cx="9688277" cy="2943636"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>187</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>496305</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>143267</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="35623500"/>
+          <a:ext cx="7201905" cy="2810267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>207</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>448844</xdr:colOff>
+      <xdr:row>217</xdr:row>
+      <xdr:rowOff>9790</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="39452550"/>
+          <a:ext cx="8373644" cy="1895740"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>220</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>77232</xdr:colOff>
+      <xdr:row>231</xdr:row>
+      <xdr:rowOff>86029</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="41910000"/>
+          <a:ext cx="7392432" cy="2181529"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>572601</xdr:colOff>
+      <xdr:row>244</xdr:row>
+      <xdr:rowOff>114582</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="44577000"/>
+          <a:ext cx="7887801" cy="2019582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>250</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>48908</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>85843</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="47625000"/>
+          <a:ext cx="9192908" cy="847843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>256</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>544192</xdr:colOff>
+      <xdr:row>261</xdr:row>
+      <xdr:rowOff>66795</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="48929925"/>
+          <a:ext cx="9078592" cy="857370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>334528</xdr:colOff>
+      <xdr:row>275</xdr:row>
+      <xdr:rowOff>19345</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="50292000"/>
+          <a:ext cx="8259328" cy="2114845"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>279</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>48738</xdr:colOff>
+      <xdr:row>293</xdr:row>
+      <xdr:rowOff>143251</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="53263800"/>
+          <a:ext cx="7973538" cy="2695951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>296</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>601010</xdr:colOff>
+      <xdr:row>301</xdr:row>
+      <xdr:rowOff>171602</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Picture 26"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="56426100"/>
+          <a:ext cx="6697010" cy="1086002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>308</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>296763</xdr:colOff>
+      <xdr:row>316</xdr:row>
+      <xdr:rowOff>9720</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Picture 27"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="58807350"/>
+          <a:ext cx="10659963" cy="1400370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>320</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>39637</xdr:colOff>
+      <xdr:row>322</xdr:row>
+      <xdr:rowOff>76255</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Picture 28"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="61026675"/>
+          <a:ext cx="11012437" cy="390580"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>323</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>248791</xdr:colOff>
+      <xdr:row>325</xdr:row>
+      <xdr:rowOff>38143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Picture 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="61645800"/>
+          <a:ext cx="8173591" cy="304843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>330</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>220042</xdr:colOff>
+      <xdr:row>333</xdr:row>
+      <xdr:rowOff>114388</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Picture 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="62922150"/>
+          <a:ext cx="6925642" cy="628738"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>337</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>591483</xdr:colOff>
+      <xdr:row>341</xdr:row>
+      <xdr:rowOff>28677</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Picture 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="64255650"/>
+          <a:ext cx="6687483" cy="733527"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>346</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>410738</xdr:colOff>
+      <xdr:row>352</xdr:row>
+      <xdr:rowOff>114475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Picture 32"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="65913000"/>
+          <a:ext cx="8335538" cy="1257475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>105811</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>133460</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1247775"/>
+          <a:ext cx="7421011" cy="790685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>420009</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>95410</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2571750"/>
+          <a:ext cx="6516009" cy="1143160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>316071</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4381500"/>
+          <a:ext cx="12508071" cy="1124107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>277965</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>123975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6096000"/>
+          <a:ext cx="12469965" cy="1076475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>354176</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>181133</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8191500"/>
+          <a:ext cx="12546176" cy="1133633"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>201244</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>133660</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="11249025"/>
+          <a:ext cx="8735644" cy="2219635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4894,11 +6246,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B28" sqref="B28"/>
+      <selection pane="bottomRight" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4911,41 +6263,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="26"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="28"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
@@ -6346,9 +7698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D162"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -6690,9 +8040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H74" sqref="H74"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -7079,7 +8427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -7166,10 +8514,10 @@
       <c r="G80" s="17"/>
     </row>
     <row r="82" spans="1:2">
-      <c r="A82" s="29" t="s">
+      <c r="A82" s="26" t="s">
         <v>227</v>
       </c>
-      <c r="B82" s="29"/>
+      <c r="B82" s="26"/>
     </row>
     <row r="83" spans="1:2">
       <c r="B83" t="s">
@@ -7177,10 +8525,10 @@
       </c>
     </row>
     <row r="95" spans="1:2">
-      <c r="A95" s="29" t="s">
+      <c r="A95" s="26" t="s">
         <v>229</v>
       </c>
-      <c r="B95" s="29"/>
+      <c r="B95" s="26"/>
     </row>
     <row r="96" spans="1:2">
       <c r="B96" t="s">
@@ -7188,10 +8536,10 @@
       </c>
     </row>
     <row r="106" spans="1:2">
-      <c r="A106" s="29" t="s">
+      <c r="A106" s="26" t="s">
         <v>231</v>
       </c>
-      <c r="B106" s="29"/>
+      <c r="B106" s="26"/>
     </row>
     <row r="107" spans="1:2">
       <c r="B107" t="s">
@@ -7199,10 +8547,10 @@
       </c>
     </row>
     <row r="117" spans="1:2">
-      <c r="A117" s="29" t="s">
+      <c r="A117" s="26" t="s">
         <v>233</v>
       </c>
-      <c r="B117" s="29"/>
+      <c r="B117" s="26"/>
     </row>
     <row r="118" spans="1:2">
       <c r="B118" t="s">
@@ -7210,13 +8558,13 @@
       </c>
     </row>
     <row r="120" spans="1:2">
-      <c r="A120" s="30"/>
+      <c r="A120" s="27"/>
     </row>
     <row r="128" spans="1:2">
-      <c r="A128" s="29" t="s">
+      <c r="A128" s="26" t="s">
         <v>235</v>
       </c>
-      <c r="B128" s="29"/>
+      <c r="B128" s="26"/>
     </row>
     <row r="129" spans="1:2">
       <c r="B129" t="s">
@@ -7224,10 +8572,10 @@
       </c>
     </row>
     <row r="143" spans="1:2">
-      <c r="A143" s="29" t="s">
+      <c r="A143" s="26" t="s">
         <v>237</v>
       </c>
-      <c r="B143" s="29"/>
+      <c r="B143" s="26"/>
     </row>
     <row r="144" spans="1:2">
       <c r="B144" t="s">
@@ -7235,10 +8583,10 @@
       </c>
     </row>
     <row r="159" spans="1:2">
-      <c r="A159" s="29" t="s">
+      <c r="A159" s="26" t="s">
         <v>239</v>
       </c>
-      <c r="B159" s="29"/>
+      <c r="B159" s="26"/>
     </row>
     <row r="160" spans="1:2">
       <c r="B160" t="s">
@@ -7254,10 +8602,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L113"/>
+  <dimension ref="A1:L345"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="M105" sqref="M105"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7416,8 +8764,309 @@
       <c r="I113" s="20"/>
       <c r="J113" s="20"/>
     </row>
+    <row r="115" spans="1:10">
+      <c r="A115" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="B115" s="17"/>
+    </row>
+    <row r="116" spans="1:10">
+      <c r="A116" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B165" s="17"/>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1">
+      <c r="A277" s="17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1">
+      <c r="A279" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7">
+      <c r="A296" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7">
+      <c r="A304" s="20" t="s">
+        <v>284</v>
+      </c>
+      <c r="B304" s="20"/>
+      <c r="C304" s="20"/>
+      <c r="D304" s="20"/>
+      <c r="E304" s="20"/>
+      <c r="F304" s="20"/>
+      <c r="G304" s="20"/>
+    </row>
+    <row r="306" spans="1:3">
+      <c r="A306" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="B306" s="17"/>
+      <c r="C306" s="17"/>
+    </row>
+    <row r="308" spans="1:3">
+      <c r="A308" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3">
+      <c r="A318" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="B318" s="17"/>
+    </row>
+    <row r="320" spans="1:3">
+      <c r="A320" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2">
+      <c r="A328" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="B328" s="17"/>
+    </row>
+    <row r="330" spans="1:2">
+      <c r="A330" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2">
+      <c r="A335" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="B335" s="17"/>
+    </row>
+    <row r="337" spans="1:2">
+      <c r="A337" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2">
+      <c r="A343" s="17" t="s">
+        <v>293</v>
+      </c>
+      <c r="B343" s="17"/>
+    </row>
+    <row r="345" spans="1:2">
+      <c r="A345" t="s">
+        <v>294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E58"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="20" t="s">
+        <v>295</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="20"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="20" t="s">
+        <v>307</v>
+      </c>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>308</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="20" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="B2" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="C2" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Done 8. Cấu trúc dữ liệu và giải thuật javascript
</commit_message>
<xml_diff>
--- a/ListHandOver/Training_User.xlsx
+++ b/ListHandOver/Training_User.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="367">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -2278,6 +2278,45 @@
   </si>
   <si>
     <t>LinkedList</t>
+  </si>
+  <si>
+    <t>Khởi tạo 1 LinkedList và Node cho LinkedList</t>
+  </si>
+  <si>
+    <t>Tạo phương thức Add cho LinkdedList để có thể thêm 1 Node mới vào LinkdedList</t>
+  </si>
+  <si>
+    <t>Tạo phương thức get để lấy 1 Node cuả LinkdedList dựa trên chỉ số truyền vào</t>
+  </si>
+  <si>
+    <t>Ta có thể lấy giá trị ở chỉ số 1 là "Item 2" với phương thức get</t>
+  </si>
+  <si>
+    <t>Tạo phương thức remove để xóa đi 1 Node của LinkedList dựa trên chỉ số truyền vào</t>
+  </si>
+  <si>
+    <t>Sau khi xóa vị trí số 2 thì node ở đây không tồn tại</t>
+  </si>
+  <si>
+    <t>Sets</t>
+  </si>
+  <si>
+    <t>là một loại object cho phép bạn lưu trữ dữ liệu một cách duy nhất, không trùng lặp.</t>
+  </si>
+  <si>
+    <t>Maps</t>
+  </si>
+  <si>
+    <t>Có thể tạo 1 mảng mới theo một điều kiện nào đó từ một tập giá trị ban đầu</t>
+  </si>
+  <si>
+    <t>Hashtable + Hashing</t>
+  </si>
+  <si>
+    <t>Hashing là phân phối các cặp khóa/giá trị trên một mảng. Nó sử dụng một hash function (hàm băm) để chuyển đổi các khóa có giá trị lớn thành giá trị nhỏ hơn và sử dụng số nhỏ hơn đó làm chỉ mục trong một bảng gọi là hash table</t>
+  </si>
+  <si>
+    <t>Khởi tạo 1 Hashtable cơ bản với 3 chức năng get, set và remove item</t>
   </si>
 </sst>
 </file>
@@ -6686,6 +6725,348 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>495709</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>133649</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="21231225"/>
+          <a:ext cx="2934109" cy="2143424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>410058</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>143409</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="23936325"/>
+          <a:ext cx="3458058" cy="3829584"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>515102</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>38770</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="28384500"/>
+          <a:ext cx="5391902" cy="4801270"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323971</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>43</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6162675" y="31127700"/>
+          <a:ext cx="866896" cy="304843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>178</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>342019</xdr:colOff>
+      <xdr:row>217</xdr:row>
+      <xdr:rowOff>113357</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="33909000"/>
+          <a:ext cx="7047619" cy="7542857"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>198</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>581191</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>104816</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7315200" y="37719000"/>
+          <a:ext cx="1190791" cy="295316"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>222</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>581532</xdr:colOff>
+      <xdr:row>235</xdr:row>
+      <xdr:rowOff>152767</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="42291000"/>
+          <a:ext cx="3629532" cy="2629267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>240</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>267843</xdr:colOff>
+      <xdr:row>252</xdr:row>
+      <xdr:rowOff>143214</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="45720000"/>
+          <a:ext cx="8192643" cy="2429214"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>361067</xdr:colOff>
+      <xdr:row>297</xdr:row>
+      <xdr:rowOff>8619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="49339500"/>
+          <a:ext cx="7066667" cy="7247619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6955,10 +7336,10 @@
   <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B36" sqref="B36"/>
+      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9914,11 +10295,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F108"/>
+  <dimension ref="A1:M258"/>
   <sheetViews>
-    <sheetView topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -10032,13 +10411,80 @@
         <v>352</v>
       </c>
     </row>
-    <row r="108" spans="2:2">
+    <row r="108" spans="1:2">
       <c r="B108" s="17" t="s">
         <v>353</v>
       </c>
     </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="163" spans="11:11">
+      <c r="K163" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="197" spans="13:13">
+      <c r="M197" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2">
+      <c r="B220" s="17" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2">
+      <c r="B221" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2">
+      <c r="B238" s="17" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2">
+      <c r="B239" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="255" spans="2:3">
+      <c r="B255" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="C255" s="17"/>
+    </row>
+    <row r="256" spans="2:3">
+      <c r="B256" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" t="s">
+        <v>366</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Done 9 Lập trình hướng đối tượng
</commit_message>
<xml_diff>
--- a/ListHandOver/Training_User.xlsx
+++ b/ListHandOver/Training_User.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="5" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ListHandOver" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,8 @@
     <sheet name="Scope của variables" sheetId="9" r:id="rId7"/>
     <sheet name="Làm việc với con trỏ this" sheetId="10" r:id="rId8"/>
     <sheet name="CTDL và giải thuật" sheetId="11" r:id="rId9"/>
+    <sheet name="Lập trình hướng đối tượng" sheetId="12" r:id="rId10"/>
+    <sheet name="Lập trình bất đồng bộ" sheetId="13" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="374">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -2317,6 +2319,27 @@
   </si>
   <si>
     <t>Khởi tạo 1 Hashtable cơ bản với 3 chức năng get, set và remove item</t>
+  </si>
+  <si>
+    <t>Encapsulation (Tính đóng gói)</t>
+  </si>
+  <si>
+    <t>che giấu dữ liệu, không cho phép truy cập dữ liệu trực tiếp từ bên ngoài, mà phải thông qua các method được cung cấp</t>
+  </si>
+  <si>
+    <t>Inheritance (Tính kế thừa)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">đối tượng con sẽ kế thừa những thuộc tính của đối tượng cha mà không cần phải định nghĩa lại. </t>
+  </si>
+  <si>
+    <t>Mặc dù, JavaScript không hỗ trợ trực tiếp tính kế thừa, tuy nhiên ta vẫn có thể tuỳ biến để áp dụng tính chất này trong JavaScript.</t>
+  </si>
+  <si>
+    <t>Polymorphism (Tính đa hình), Abstraction (Tính trừa tượng)</t>
+  </si>
+  <si>
+    <t>Javascript không có class và Interface nên tính chất này không được thể hiện. Tuy nhiên Typescript đã có và thể hiện được tính 2 chất này.</t>
   </si>
 </sst>
 </file>
@@ -7070,6 +7093,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>343543</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9819</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="4610743" cy="2105319"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>39637</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>29091</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3571875"/>
+          <a:ext cx="11012437" cy="3696216"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7335,11 +7439,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D69" sqref="D69"/>
+      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8783,6 +8887,79 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="20" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="20" t="s">
+        <v>369</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="B41" t="s">
+        <v>373</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D162"/>

</xml_diff>

<commit_message>
Done 11/ Exception handling
</commit_message>
<xml_diff>
--- a/ListHandOver/Training_User.xlsx
+++ b/ListHandOver/Training_User.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="5" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="ListHandOver" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="CTDL và giải thuật" sheetId="11" r:id="rId9"/>
     <sheet name="Lập trình hướng đối tượng" sheetId="12" r:id="rId10"/>
     <sheet name="Lập trình bất đồng bộ" sheetId="13" r:id="rId11"/>
+    <sheet name="Exception handling" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="396">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -2340,6 +2341,72 @@
   </si>
   <si>
     <t>Javascript không có class và Interface nên tính chất này không được thể hiện. Tuy nhiên Typescript đã có và thể hiện được tính 2 chất này.</t>
+  </si>
+  <si>
+    <t>Call back</t>
+  </si>
+  <si>
+    <t xml:space="preserve">là một hàm sẽ được thực hiện sau khi một hàm khác đã thực hiện xong </t>
+  </si>
+  <si>
+    <t>Callback là một cách để đảm bảo code nhất định không thực thi cho đến khi code khác thực hiện xong</t>
+  </si>
+  <si>
+    <t>Giả sử ta có quy trình gửi mail như bên dưới</t>
+  </si>
+  <si>
+    <t>Và sẽ không có vấn đề nếu tiến trình gửi mail không lâu</t>
+  </si>
+  <si>
+    <t>Tuy nhiên nếu gửi mail quá lâu thì việc đợi để thông báo thành công sẽ diễn ra sau. Như này</t>
+  </si>
+  <si>
+    <t>Ta có thể dùng call back để đợi wait() chạy xong mới thực hiện end()</t>
+  </si>
+  <si>
+    <t>Promise</t>
+  </si>
+  <si>
+    <t>là một cơ chế trong JavaScript giúp bạn thực thi các tác vụ bất đồng bộ mà không rơi vào tình trạng các hàm callback lồng vào nhau ở quá nhiều tầng.</t>
+  </si>
+  <si>
+    <t>resolve sẽ dùng để gọi khi thao tác xử lý thành công</t>
+  </si>
+  <si>
+    <t>reject sẽ dùng để gọi khi thao tác xử lý thất bại</t>
+  </si>
+  <si>
+    <t>Async/await</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vậy để tránh viết như minh họa bên dưới </t>
+  </si>
+  <si>
+    <t>Ta có thể viết với Promise dạng như sau</t>
+  </si>
+  <si>
+    <t>Async - khai báo một hàm bất đồng bộ</t>
+  </si>
+  <si>
+    <t>Await - tạm dừng việc thực hiện các hàm async</t>
+  </si>
+  <si>
+    <t>Giả sử các hàm getValue là các API giá trị trả về là bất đồng bộ ta có thể viết như sau</t>
+  </si>
+  <si>
+    <t>Exception handling</t>
+  </si>
+  <si>
+    <t>Để có thể xử lý lỗi ngoại lệ ta có thể xem ví dụ sau</t>
+  </si>
+  <si>
+    <t>Trong try sẽ là xử lý để lấy ra thông tin người dùng</t>
+  </si>
+  <si>
+    <t>Trường hợp một lỗi nào đó phát sinh trong quá trình lấy thông tin thì catch sẽ được thực thi</t>
+  </si>
+  <si>
+    <t>Finally được can thiệp ở trường hợp này là nếu quá trình lấy thông tin lỗi thì hasErr, nên giá trị hasUser được set lại false</t>
   </si>
 </sst>
 </file>
@@ -3030,6 +3097,451 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>268099</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>322</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1314450"/>
+          <a:ext cx="10021699" cy="2305372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>191888</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>19425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4191000"/>
+          <a:ext cx="9945488" cy="2686425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>591909</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>143241</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7429500"/>
+          <a:ext cx="9735909" cy="2619741"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>9867</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="10858500"/>
+          <a:ext cx="2448267" cy="2857899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>57315</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>19119</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3143250" y="12096750"/>
+          <a:ext cx="1181265" cy="495369"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>1361</xdr:colOff>
+      <xdr:row>90</xdr:row>
+      <xdr:rowOff>86144</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="14230350"/>
+          <a:ext cx="9754961" cy="3000794"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Avoiding Callback Hell with Async.js"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="17830800"/>
+          <a:ext cx="6076950" cy="4562475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>552782</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>134033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="23050500"/>
+          <a:ext cx="2381582" cy="4896533"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419282</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>28750</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2771775" y="24869775"/>
+          <a:ext cx="1305107" cy="1257475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>514762</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>47932</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="29660850"/>
+          <a:ext cx="2953162" cy="2200582"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371952</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>105135</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="3419952" cy="2581635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -7439,11 +7951,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B55" sqref="B55"/>
+      <selection pane="bottomRight" activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8891,9 +9403,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U30" sqref="U30"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -8950,13 +9460,144 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="20" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="20" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="B56" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="F63" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="74" spans="6:6">
+      <c r="F74" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="20" t="s">
+        <v>385</v>
+      </c>
+      <c r="B149" s="20"/>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" t="s">
+        <v>390</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="20" t="s">
+        <v>391</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="B2" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="G5" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="G6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="G7" t="s">
+        <v>395</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Done 19/ Event Loop
</commit_message>
<xml_diff>
--- a/ListHandOver/Training_User.xlsx
+++ b/ListHandOver/Training_User.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" firstSheet="13" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="ListHandOver" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,9 @@
     <sheet name="Khái niệm chuyên sâu" sheetId="17" r:id="rId15"/>
     <sheet name="Tìm hiểu clean code" sheetId="18" r:id="rId16"/>
     <sheet name="Tìm hiểu design pattern" sheetId="19" r:id="rId17"/>
+    <sheet name="Lập trình hướng function" sheetId="20" r:id="rId18"/>
+    <sheet name="Workers" sheetId="21" r:id="rId19"/>
+    <sheet name="Event Loop " sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="563">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1"/>
@@ -446,60 +449,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>i: while..., do...while, for, forEach, for in, for of,...</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>18/ Workers</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">19/ Event Loop </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>17/ L</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ậ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p trình h</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>ướ</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="3"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>ng function</t>
     </r>
     <phoneticPr fontId="1"/>
   </si>
@@ -2759,6 +2708,207 @@
       </rPr>
       <t>u design pattern</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Design pattern là một thuật ngữ được sử dụng trong ngành kỹ nghệ phần mềm nói chung, </t>
+  </si>
+  <si>
+    <t>là giải pháp tái sử dụng cho việc giải quyết các vấn đề giống nhau và thường xuyên ra trong quá trình phát triển phần mềm</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>được sử dụng để duy trì các phần code cụ thể độc lập, không phụ thuộc vào các thành phần khác</t>
+  </si>
+  <si>
+    <t>Ví dụ</t>
+  </si>
+  <si>
+    <t>Prototype</t>
+  </si>
+  <si>
+    <t>Từ đối tượng Student ban đầu với các thuộc tính name và age ta có thể định nghĩa showHobbies cho đối tượng student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Singleton Pattern </t>
+  </si>
+  <si>
+    <t>mẫu design pattern chỉ cho phép chúng tạo ra một instantiation duy nhất của một Class.</t>
+  </si>
+  <si>
+    <t>Singleton giúp hạn chế  tạo nhiều đối tượng, sau khi đối tượng đầu tiên được tạo, nó sẽ trả về instant đã tạo của chính nó</t>
+  </si>
+  <si>
+    <t>Ngoài ra còn một số Design pattern khác</t>
+  </si>
+  <si>
+    <r>
+      <t>17/ L</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ậ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p trình h</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ướ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng function</t>
+    </r>
+  </si>
+  <si>
+    <t>là một phương pháp lập trình dựa trên các hàm toán học (function), tránh việc thay đổi giá trị của dữ liệu.</t>
+  </si>
+  <si>
+    <t>Lập trình hướng function</t>
+  </si>
+  <si>
+    <t>Ưu điểm</t>
+  </si>
+  <si>
+    <t>hướng đến tính kết hợp (composability) các hàm (function) để tối đa hóa khả năng tái sử dụng (reusability) trong chương trình</t>
+  </si>
+  <si>
+    <t>thay vì thực hiện tuần tự theo các bước với các biến để lưu trạng thái. Thì Functional Programming chú trọng đến thực thi luồng chương trình thông qua sự kết hợp các hàm bậc cao (high order function).</t>
+  </si>
+  <si>
+    <t>Nhược điểm</t>
+  </si>
+  <si>
+    <t>yêu cầu không gian bộ nhớ lớn. Vì nó không tạo ra một đơn vị mới. Cho nên mỗi lần khi sử dụng bạn cần tạo các đối tượng mới để thực hiện các hành động.</t>
+  </si>
+  <si>
+    <t>Trong một số tình huống khi mà chúng ta sử dụng lập trình hàm thì phải thực hiện nhiều thao tác khác nhau trên cùng một tập dữ liệu</t>
+  </si>
+  <si>
+    <t>Làm quen với lập trình hướng function</t>
+  </si>
+  <si>
+    <t>Pure function(Hàm thuần khiết)</t>
+  </si>
+  <si>
+    <t>Với các inputs giống nhau, luôn cho ra một output giống nhau, và không có hiệu ứng phụ</t>
+  </si>
+  <si>
+    <t>Đây là 1 hàm không thuần khiết vì nó sử dụng biến b ở bên ngoài</t>
+  </si>
+  <si>
+    <t>Sau khi biến hình mượn 1 biến c thì ta đã có 1 hàm thuần khiết</t>
+  </si>
+  <si>
+    <t>Function Composition(Sự tổng hợp của các hàm)</t>
+  </si>
+  <si>
+    <t>Là một tiến trình kết hợp hai hay nhiều hàm để tạo nên hàm mới hoặc thực hiện một nhiệm vụ gì đó.</t>
+  </si>
+  <si>
+    <t>Shared State(Biến chia sẻ)</t>
+  </si>
+  <si>
+    <t>Một shared scope bao gồm scope toàn cục và scope closure. Chúng được dùng chung quá nhiều nơi và rất khó để biết hàm nào đã làm thay đổi biến đó.</t>
+  </si>
+  <si>
+    <t>là bất cứ các biến, đối tượng, hoặc không gian bộ nhớ mà chúng tồn tại trong một pham vi được chia sẻ(shared scope).</t>
+  </si>
+  <si>
+    <t>Các hàm không nên chia sẻ nhau giữa các biến, dữ liệu.</t>
+  </si>
+  <si>
+    <t>Side Effects</t>
+  </si>
+  <si>
+    <t>là tất cả những thay đổi của state trong ứng dụng mà nó nằm bên ngoài hàm đang thực thi</t>
+  </si>
+  <si>
+    <t>18/ Workers</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>Worker Detection</t>
+  </si>
+  <si>
+    <t>Do Worker constructor function được truy cập thông qua window object, chúng ta có thể kiểm tra như sau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kiểm tra xem trình duyệt hiện tại có hỗ trợ Worker hay không. </t>
+  </si>
+  <si>
+    <t>Create New Worker</t>
+  </si>
+  <si>
+    <t>Stop New Worker</t>
+  </si>
+  <si>
+    <t>w.terminate();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19/ Event Loop </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Event Loop </t>
+  </si>
+  <si>
+    <t>là một Queue, tất cả cá event được push vào Queue này, mỗi khi một sự kiện được phát ra nó sẽ được push vào Queue.</t>
+  </si>
+  <si>
+    <t>Trong Queue này, thứ tự thực hiện là vào trước thì sẽ được xử lí trước, vào sau thì được xử lí sau.</t>
+  </si>
+  <si>
+    <t>B1: hàm main được push vào trong Call Stack. Sau đó dòng lệnh console.log(‘A’) cũng được thêm vào Stack và được thực thi in ra A.</t>
+  </si>
+  <si>
+    <t>Sau đó, console.log(‘A’) được xóa khỏi Stack.</t>
+  </si>
+  <si>
+    <t>B2: Sau đó, hàm setTimeout được push vào Stack với một callback và timer là 2000ms.</t>
+  </si>
+  <si>
+    <t>setTimeout là một Browser APIs, nên được giao lại cho Browser xử lí timer này. Callback của setTimeout được Web APIs giữ cho tới khi đúng với số thời gian timeout, ở đây là 2000ms.</t>
+  </si>
+  <si>
+    <t>Callback này sẽ tự động được push vào Event Queue sau 2000ms nữa. setTimeout được xóa khỏi Stack.</t>
+  </si>
+  <si>
+    <t>B3: console.log(‘C’) được push vào Stack và được thực thi(invoke), in ra C. Sau đó, console.log(‘C’) được xóa khỏi Stack.</t>
+  </si>
+  <si>
+    <t>B4: Tiếp theo, hàm main đã thực thi xong và cũng được xóa khỏi Stack. Lúc này, Event Loop đã nhận callback exec() của setTimeout được chờ xử lý từ bước 2.</t>
+  </si>
+  <si>
+    <t>B5: lúc này Event Loop có một callback exec(), nó sẽ được push vào Stack và in ra B. Sau đó, exec() của setTimeout cũng được xóa khỏi Stack.</t>
   </si>
 </sst>
 </file>
@@ -3077,6 +3227,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3086,7 +3237,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4974,6 +5124,444 @@
         <a:xfrm>
           <a:off x="2457450" y="3371850"/>
           <a:ext cx="1600423" cy="666843"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing16.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>181426</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28712</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1143000"/>
+          <a:ext cx="3229426" cy="981212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1021</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>162320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2667000"/>
+          <a:ext cx="7316221" cy="2829320"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438722</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>76523</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="6334125"/>
+          <a:ext cx="4096322" cy="2314898"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>134049</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>10191</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="9715500"/>
+          <a:ext cx="5010849" cy="4772691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571702</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>133491</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5219700" y="11315700"/>
+          <a:ext cx="1448002" cy="1009791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing17.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>143320</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>105002</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="3191320" cy="1629002"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>305268</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4953000"/>
+          <a:ext cx="3353268" cy="1467055"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>134305</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>133581</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="7239000"/>
+          <a:ext cx="6839905" cy="1657581"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>581957</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>133475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="952500"/>
+          <a:ext cx="6677957" cy="895475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114997</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>67110</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2476500"/>
+          <a:ext cx="4991797" cy="3115110"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>543767</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>162107</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="762000"/>
+          <a:ext cx="6030167" cy="1305107"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9394,11 +9982,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B72" sqref="B72"/>
+      <selection pane="bottomRight" activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9411,41 +9999,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="29" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="5"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="29"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9">
@@ -9470,7 +10058,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C4" s="12"/>
       <c r="D4" s="10"/>
@@ -9774,7 +10362,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="10"/>
@@ -9790,7 +10378,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="10"/>
@@ -9822,7 +10410,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="10"/>
@@ -9870,7 +10458,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="10"/>
@@ -10014,7 +10602,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C38" s="12"/>
       <c r="D38" s="10"/>
@@ -10030,7 +10618,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C39" s="12"/>
       <c r="D39" s="10"/>
@@ -10398,7 +10986,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C62" s="12"/>
       <c r="D62" s="10"/>
@@ -10542,7 +11130,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C71" s="12"/>
       <c r="D71" s="10"/>
@@ -10558,7 +11146,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C72" s="12"/>
       <c r="D72" s="10"/>
@@ -10574,7 +11162,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>81</v>
+        <v>521</v>
       </c>
       <c r="C73" s="12"/>
       <c r="D73" s="10"/>
@@ -10590,7 +11178,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>79</v>
+        <v>543</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="10"/>
@@ -10606,7 +11194,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>80</v>
+        <v>551</v>
       </c>
       <c r="C75" s="12"/>
       <c r="D75" s="10"/>
@@ -10622,7 +11210,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="10"/>
@@ -10852,36 +11440,36 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="20" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="20" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B16" s="20"/>
       <c r="C16" s="20"/>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="20" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -10891,7 +11479,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="B41" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
@@ -10911,88 +11499,88 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="20" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="20" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="B56" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="F63" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="74" spans="6:6">
       <c r="F74" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" s="20" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B149" s="20"/>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -11014,28 +11602,28 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="20" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="G5" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="G6" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="G7" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -11056,44 +11644,44 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="20" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" s="17" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C2" s="17"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -11112,32 +11700,32 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="20" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="B3" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -11157,384 +11745,384 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="20" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="B2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="G29" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="34" spans="1:19">
       <c r="A34" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="37" spans="1:19">
       <c r="S37" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="45" spans="1:19">
       <c r="J45" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" s="20" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="B72" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="B86" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="B87" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" s="20" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="B90" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="B101" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="20" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B117" s="20"/>
     </row>
     <row r="118" spans="1:2">
       <c r="B118" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" s="20" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B148" s="20"/>
     </row>
     <row r="149" spans="1:2">
       <c r="B149" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" s="21" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" s="21" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" s="21" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" s="20" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B192" s="20"/>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" s="21" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="B194" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="B195" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" s="21" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="B197" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="198" spans="1:3">
-      <c r="B198" s="31" t="s">
-        <v>457</v>
+      <c r="B198" s="28" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" s="21" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="B200" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="B201" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="20" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B206" s="20"/>
       <c r="C206" s="20"/>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="211" spans="1:2">
       <c r="A211" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="212" spans="1:2">
       <c r="A212" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="213" spans="1:2">
       <c r="A213" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="214" spans="1:2">
       <c r="A214" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="216" spans="1:2">
       <c r="A216" s="21" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="217" spans="1:2">
       <c r="B217" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="218" spans="1:2">
       <c r="B218" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="219" spans="1:2">
       <c r="B219" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="20" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B230" s="20"/>
       <c r="C230" s="20"/>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="B234" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="C235" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="C236" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="C237" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
   </sheetData>
@@ -11548,19 +12136,19 @@
   <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="20" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="B2" s="17" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
@@ -11568,137 +12156,137 @@
     </row>
     <row r="3" spans="1:8">
       <c r="B3" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="H5" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="H6" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="B9" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="E11" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="C14" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="B16" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="B18" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="D21" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="20" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="B25" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="C26" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="C27" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="B29" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="C30" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="C31" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="B33" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="C34" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="B36" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="C37" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="B39" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="C40" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="C41" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="C44" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -11709,15 +12297,260 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="20" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="B5" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="20" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="B32" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="20" t="s">
+        <v>517</v>
+      </c>
+      <c r="B48" s="20"/>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
+      <c r="B50" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>520</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G55"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="20" t="s">
+        <v>523</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="17" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="17" t="s">
+        <v>527</v>
+      </c>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="B10" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="17" t="s">
+        <v>530</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="B15" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="19" spans="7:7">
+      <c r="G19" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="28" spans="7:7">
+      <c r="G28" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="17" t="s">
+        <v>535</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="B37" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="17" t="s">
+        <v>537</v>
+      </c>
+      <c r="B49" s="17"/>
+      <c r="C49" s="17"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="B50" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="B51" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="B52" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" s="17" t="s">
+        <v>541</v>
+      </c>
+      <c r="B54" s="17"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="B55" t="s">
+        <v>542</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="20" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="17" t="s">
+        <v>545</v>
+      </c>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" s="17" t="s">
+        <v>548</v>
+      </c>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="31" spans="2:3">
+      <c r="B31" s="17" t="s">
+        <v>549</v>
+      </c>
+      <c r="C31" s="17"/>
+    </row>
+    <row r="32" spans="2:3">
+      <c r="C32" t="s">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11731,134 +12564,134 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="20" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" s="17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="B8" s="18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="B14" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="B16" s="17" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="B20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="B21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="B29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="B35" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="18" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="B39" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="B40" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="B48" s="17" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="B65" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="18" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B77" s="19"/>
       <c r="C77" s="19"/>
@@ -11866,200 +12699,270 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="B81" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="B82" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="B83" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="B90" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="B91" s="18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="B92" s="18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="C93" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" s="21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="B96" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="C97" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="C98" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="C99" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="C100" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="C101" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" s="21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="B104" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="B105" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="B106" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="B107" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="B108" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" s="21" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="B111" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="B112" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="B113" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="B114" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" s="21" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" s="20" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B118" s="16"/>
       <c r="C118" s="16"/>
     </row>
     <row r="119" spans="1:3">
       <c r="B119" s="17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="136" spans="2:2">
       <c r="B136" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="137" spans="2:2">
       <c r="B137" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="162" spans="2:2">
       <c r="B162" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="20" t="s">
+        <v>552</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="B2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -12073,133 +12976,133 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:3">
       <c r="B2" s="17" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="B3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="B10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="B15" s="17" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C15" s="17"/>
     </row>
     <row r="17" spans="1:6">
       <c r="F17" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="F20" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="20" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B27" s="16"/>
     </row>
     <row r="28" spans="1:6">
       <c r="B28" s="17" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="C29" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="2:3">
       <c r="B44" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="C45" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="B77" s="21" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="20" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B80" s="16"/>
       <c r="C80" s="16"/>
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="G85" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:7">
       <c r="A94" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B94" s="16"/>
     </row>
     <row r="95" spans="1:7">
       <c r="B95" s="17" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="2:3">
       <c r="B105" s="17" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C105" s="17"/>
     </row>
@@ -12220,130 +13123,130 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="20" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="20" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="J24" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="22" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="B36" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="B48" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="20" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="B58" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="70" spans="1:11">
       <c r="A70" s="20" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B70" s="20"/>
       <c r="C70" s="20"/>
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="B73" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="K76" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="K77" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="2:14">
       <c r="B84" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="87" spans="2:14">
       <c r="N87" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="2:14">
       <c r="N88" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="89" spans="2:14">
       <c r="N89" s="21" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="2:14">
       <c r="N90" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="91" spans="2:14">
       <c r="N91" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="158" spans="1:4">
       <c r="A158" s="20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B158" s="20"/>
       <c r="C158" s="20"/>
@@ -12351,53 +13254,53 @@
     </row>
     <row r="159" spans="1:4">
       <c r="A159" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="160" spans="1:4">
       <c r="B160" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="B166" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="B172" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="B176" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="180" spans="1:4">
       <c r="B180" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="186" spans="1:4">
       <c r="A186" s="24" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="187" spans="1:4">
       <c r="A187" s="23"/>
       <c r="B187" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="189" spans="1:4">
       <c r="A189" s="20" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B189" s="20"/>
       <c r="C189" s="20"/>
@@ -12405,42 +13308,42 @@
     </row>
     <row r="191" spans="1:4">
       <c r="A191" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="192" spans="1:4">
       <c r="A192" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="226" spans="2:2">
       <c r="B226" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="264" spans="2:2">
       <c r="B264" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="283" spans="2:2">
       <c r="B283" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="303" spans="2:2">
       <c r="B303" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -12460,7 +13363,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="20" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -12474,45 +13377,45 @@
     </row>
     <row r="2" spans="1:10">
       <c r="B2" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:10">
       <c r="B3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="C4" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="17" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C13" s="17"/>
     </row>
     <row r="14" spans="1:10">
       <c r="B14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="C16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="17" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -12522,7 +13425,7 @@
     </row>
     <row r="62" spans="2:7">
       <c r="B62" s="17" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="17"/>
@@ -12532,7 +13435,7 @@
     </row>
     <row r="80" spans="2:7">
       <c r="B80" s="17" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C80" s="17"/>
       <c r="D80" s="17"/>
@@ -12542,46 +13445,46 @@
     </row>
     <row r="82" spans="1:2">
       <c r="A82" s="26" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B82" s="26"/>
     </row>
     <row r="83" spans="1:2">
       <c r="B83" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" s="26" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B95" s="26"/>
     </row>
     <row r="96" spans="1:2">
       <c r="B96" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" s="26" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B106" s="26"/>
     </row>
     <row r="107" spans="1:2">
       <c r="B107" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" s="26" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B117" s="26"/>
     </row>
     <row r="118" spans="1:2">
       <c r="B118" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -12589,35 +13492,35 @@
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="26" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B128" s="26"/>
     </row>
     <row r="129" spans="1:2">
       <c r="B129" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" s="26" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B143" s="26"/>
     </row>
     <row r="144" spans="1:2">
       <c r="B144" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" s="26" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B159" s="26"/>
     </row>
     <row r="160" spans="1:2">
       <c r="B160" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -12639,7 +13542,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="20" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -12649,29 +13552,29 @@
     </row>
     <row r="2" spans="1:6">
       <c r="B2" s="17" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C2" s="17"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="17" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C10" s="17"/>
     </row>
     <row r="19" spans="1:12">
       <c r="B19" s="17" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="27" spans="1:12">
       <c r="B27" s="17" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -12686,7 +13589,7 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" s="20" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B29" s="20"/>
       <c r="C29" s="20"/>
@@ -12699,87 +13602,87 @@
     </row>
     <row r="31" spans="1:12">
       <c r="B31" s="17" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="C32" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="45" spans="2:3">
       <c r="B45" s="17" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="46" spans="2:3">
       <c r="C46" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="56" spans="2:3">
       <c r="B56" s="17" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="57" spans="2:3">
       <c r="C57" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="B67" s="17" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="C68" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="78" spans="2:3">
       <c r="B78" s="17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="C79" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="B88" s="17" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="2:3">
       <c r="C89" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="97" spans="2:3">
       <c r="B97" s="17" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="98" spans="2:3">
       <c r="C98" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="106" spans="2:3">
       <c r="B106" s="17" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="107" spans="2:3">
       <c r="C107" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="113" spans="1:10">
       <c r="A113" s="20" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B113" s="20"/>
       <c r="C113" s="20"/>
@@ -12793,99 +13696,99 @@
     </row>
     <row r="115" spans="1:10">
       <c r="A115" s="17" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B115" s="17"/>
     </row>
     <row r="116" spans="1:10">
       <c r="A116" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" s="17" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B165" s="17"/>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" s="17" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="247" spans="1:1">
       <c r="A247" s="17" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="249" spans="1:1">
       <c r="A249" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="256" spans="1:1">
       <c r="A256" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="263" spans="1:1">
       <c r="A263" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="277" spans="1:1">
       <c r="A277" s="17" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="279" spans="1:1">
       <c r="A279" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="296" spans="1:7">
       <c r="A296" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="304" spans="1:7">
       <c r="A304" s="20" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B304" s="20"/>
       <c r="C304" s="20"/>
@@ -12896,58 +13799,58 @@
     </row>
     <row r="306" spans="1:3">
       <c r="A306" s="17" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B306" s="17"/>
       <c r="C306" s="17"/>
     </row>
     <row r="308" spans="1:3">
       <c r="A308" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="318" spans="1:3">
       <c r="A318" s="17" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B318" s="17"/>
     </row>
     <row r="320" spans="1:3">
       <c r="A320" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="328" spans="1:2">
       <c r="A328" s="17" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B328" s="17"/>
     </row>
     <row r="330" spans="1:2">
       <c r="A330" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="335" spans="1:2">
       <c r="A335" s="17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B335" s="17"/>
     </row>
     <row r="337" spans="1:2">
       <c r="A337" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="343" spans="1:2">
       <c r="A343" s="17" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B343" s="17"/>
     </row>
     <row r="345" spans="1:2">
       <c r="A345" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -12969,18 +13872,18 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="20" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B1" s="20"/>
     </row>
     <row r="2" spans="1:5">
       <c r="B2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="20" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -12989,27 +13892,27 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="20" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B40" s="20"/>
       <c r="C40" s="20"/>
@@ -13017,12 +13920,12 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="20" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B51" s="20"/>
       <c r="C51" s="20"/>
@@ -13030,17 +13933,17 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="20" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B56" s="20"/>
       <c r="C56" s="20"/>
@@ -13049,7 +13952,7 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -13070,7 +13973,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="20" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -13089,7 +13992,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="20" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -13099,97 +14002,97 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3" s="17" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C3" s="17"/>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="B14" s="17" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C14" s="17"/>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="B37" s="17" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C37" s="17"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="B92" s="17" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C92" s="17"/>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="B104" s="17" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C104" s="17"/>
     </row>
     <row r="105" spans="1:3">
       <c r="B105" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="113" spans="1:8">
       <c r="A113" s="20" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B113" s="20"/>
       <c r="C113" s="20"/>
@@ -13201,27 +14104,27 @@
     </row>
     <row r="115" spans="1:8">
       <c r="B115" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:8">
       <c r="A116" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="118" spans="1:8">
       <c r="B118" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="121" spans="1:8">
       <c r="A121" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -13243,7 +14146,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="20" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
@@ -13251,175 +14154,175 @@
     </row>
     <row r="3" spans="1:4">
       <c r="B3" s="17" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C3" s="17"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="B43" s="17" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C43" s="17"/>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="B47" s="17" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="F59" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="B77" s="17" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="F91" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="B108" s="17" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="163" spans="11:11">
       <c r="K163" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="197" spans="13:13">
       <c r="M197" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="220" spans="2:2">
       <c r="B220" s="17" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="221" spans="2:2">
       <c r="B221" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="238" spans="2:2">
       <c r="B238" s="17" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="239" spans="2:2">
       <c r="B239" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="255" spans="2:3">
       <c r="B255" s="17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C255" s="17"/>
     </row>
     <row r="256" spans="2:3">
       <c r="B256" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="258" spans="1:1">
       <c r="A258" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
   </sheetData>

</xml_diff>